<commit_message>
Forgot to use ExcelWriter.
</commit_message>
<xml_diff>
--- a/SET100.xlsx
+++ b/SET100.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="StocksAdd" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UpdateSeq" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="StocksAdd" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,6 +427,572 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>update_seq</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>date_from</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>date_to</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>date_published</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Update_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2014-01-01</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2014-06-30</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2013-12-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Update_2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2014-07-01</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2014-12-31</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2020-11-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Update_3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2015-01-01</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2015-06-30</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2020-11-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Update_4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2015-01-01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2015-06-30</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2015-04-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Update_5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2015-07-01</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2015-12-31</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2015-06-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Update_6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2016-01-01</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2016-06-30</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2015-12-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Update_7</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2016-01-01</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2016-06-30</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2015-12-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Update_8</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2016-12-31</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2016-06-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Update_9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2016-07-01</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2016-12-31</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2016-12-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Update_10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2017-01-01</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2017-06-30</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2016-12-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Update_11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2017-07-01</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2017-12-31</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2017-06-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Update_12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2018-01-01</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2018-06-30</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2017-12-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Update_13</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2018-07-01</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2018-12-31</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2018-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Update_14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2019-01-01</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2019-06-30</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2018-12-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Update_15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2019-01-01</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2019-06-30</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2019-05-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Update_16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2019-07-01</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2019-12-31</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2019-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Update_17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2019-07-01</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2019-12-31</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2019-10-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Update_18</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2020-01-01</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2020-06-30</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2019-12-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Update_19</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2020-01-01</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2020-06-30</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2020-02-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Update_20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2020-07-01</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2020-12-31</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2020-06-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Update_21</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2020-07-01</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2020-12-31</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2020-10-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>